<commit_message>
Added data as md
</commit_message>
<xml_diff>
--- a/Data/CV/Plots_CV.xlsx
+++ b/Data/CV/Plots_CV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Files\My Drive\Study_Stuff\Semester-8\Integrated_Laborotary_II\Experiment_1_LockInAmplifier_using_Expeyes\Codes_for_Expeyes\Data\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0651636B-FF5B-4AA3-B78A-CF8E50556E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE10B8F-0EAB-42E8-BBE7-EC679BA68491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{D83F0066-2F64-4B59-AAE8-191E747E93A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{D83F0066-2F64-4B59-AAE8-191E747E93A3}"/>
   </bookViews>
   <sheets>
     <sheet name="PolyCrystalline(Small)" sheetId="4" state="hidden" r:id="rId1"/>
@@ -444,6 +444,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -454,9 +457,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11021,16 +11021,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
@@ -11686,8 +11686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AC2DB2-A0C7-4A7E-824B-304053C1C4EF}">
   <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11702,16 +11702,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
@@ -11749,25 +11749,25 @@
       <c r="B4" s="2">
         <v>0.2</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="15">
         <v>1.9997463329354884E-3</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="15">
         <v>3.8811468124265475E-2</v>
       </c>
       <c r="E4" s="2">
         <v>0.2</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="15">
         <v>3.769880976343537E-3</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="15">
         <v>7.3333990142910588E-2</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="15">
         <v>2.942606336644245</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="15">
         <v>0.11548768300081896</v>
       </c>
     </row>
@@ -11775,25 +11775,25 @@
       <c r="B5" s="2">
         <v>0.3</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="15">
         <v>1.999303942313548E-3</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="15">
         <v>3.8842882845335991E-2</v>
       </c>
       <c r="E5" s="2">
         <v>0.3</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="15">
         <v>4.7280100874207871E-3</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="15">
         <v>9.0324104125940274E-2</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="15">
         <v>2.3909075474370813</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="15">
         <v>0.17493408351333833</v>
       </c>
     </row>
@@ -11801,25 +11801,25 @@
       <c r="B6" s="2">
         <v>0.4</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="15">
         <v>1.989384123494667E-3</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <v>3.8600184904564599E-2</v>
       </c>
       <c r="E6" s="2">
         <v>0.4</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <v>6.2240158467049894E-3</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <v>0.1212988161567181</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="15">
         <v>1.7693455351143605</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="15">
         <v>0.31942925682342299</v>
       </c>
     </row>
@@ -11827,25 +11827,25 @@
       <c r="B7" s="2">
         <v>0.5</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="15">
         <v>1.9837997933919941E-3</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="15">
         <v>3.8474951502813749E-2</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <v>6.9777045985114344E-3</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="15">
         <v>0.1349970849794726</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="15">
         <v>1.5846218445427895</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="15">
         <v>0.39824352460090162</v>
       </c>
     </row>
@@ -11853,25 +11853,25 @@
       <c r="B8" s="2">
         <v>0.6</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="15">
         <v>2.0023850545011061E-3</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="15">
         <v>3.8881937244317225E-2</v>
       </c>
       <c r="E8" s="2">
         <v>0.6</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <v>8.2350223569499607E-3</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="15">
         <v>0.15860032238019833</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="15">
         <v>1.3630415197500503</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="15">
         <v>0.53824726256012234</v>
       </c>
     </row>
@@ -11879,25 +11879,25 @@
       <c r="B9" s="2">
         <v>0.7</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="15">
         <v>1.996412815259121E-3</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <v>3.8725354693569906E-2</v>
       </c>
       <c r="E9" s="2">
         <v>0.7</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <v>9.9529682427608943E-3</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="15">
         <v>0.19370694167090247</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="15">
         <v>1.1115495553472912</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="15">
         <v>0.80936112647757252</v>
       </c>
     </row>
@@ -11905,25 +11905,25 @@
       <c r="B10" s="2">
         <v>0.8</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <v>1.9988664639107815E-3</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="15">
         <v>3.8803647087173383E-2</v>
       </c>
       <c r="E10" s="2">
         <v>0.8</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <v>1.0900906066803547E-2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="15">
         <v>0.21327338770198115</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="15">
         <v>1.011624935143463</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="15">
         <v>0.97714935318660356</v>
       </c>
     </row>
@@ -11931,25 +11931,25 @@
       <c r="B11" s="2">
         <v>0.9</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="15">
         <v>2.0009446226472989E-3</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="15">
         <v>3.8834949954710769E-2</v>
       </c>
       <c r="E11" s="2">
         <v>0.9</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <v>1.3359958046020796E-2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="15">
         <v>0.25945972242517695</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="15">
         <v>0.83220117655741499</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="15">
         <v>1.4439207219766785</v>
       </c>
     </row>
@@ -11957,25 +11957,25 @@
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="15">
         <v>1.999501369459129E-3</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="15">
         <v>3.8827166987648452E-2</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <v>1.5060839552766306E-2</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="15">
         <v>0.2903715086458496</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="15">
         <v>0.74344386484269198</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="15">
         <v>1.8092710589623222</v>
       </c>
     </row>
@@ -11983,25 +11983,25 @@
       <c r="B13" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="15">
         <v>2.0023371201207908E-3</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="15">
         <v>3.8874078560465812E-2</v>
       </c>
       <c r="E13" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>1.6938231633672883E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>0.32827991596378203</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="15">
         <v>0.6583981549630461</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="15">
         <v>2.3068682386798911</v>
       </c>
     </row>
@@ -12009,25 +12009,25 @@
       <c r="B14" s="2">
         <v>1.2</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="15">
         <v>1.991147076137228E-3</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="15">
         <v>3.8592252849558195E-2</v>
       </c>
       <c r="E14" s="2">
         <v>1.2</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="15">
         <v>1.897866366778796E-2</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="15">
         <v>0.36619813877544327</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="15">
         <v>0.58594059600615134</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="15">
         <v>2.9126803306949585</v>
       </c>
     </row>
@@ -12035,25 +12035,25 @@
       <c r="B15" s="2">
         <v>1.3</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="15">
         <v>2.0037806376779791E-3</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="15">
         <v>3.8874032126811328E-2</v>
       </c>
       <c r="E15" s="2">
         <v>1.3</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="15">
         <v>2.0371853546541818E-2</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="15">
         <v>0.39524321495469483</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="15">
         <v>0.54685227401245162</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="15">
         <v>3.3439513867127659</v>
       </c>
     </row>
@@ -12061,25 +12061,25 @@
       <c r="B16" s="2">
         <v>1.4</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="15">
         <v>2.0003921959662932E-3</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="15">
         <v>3.8827124468188076E-2</v>
       </c>
       <c r="E16" s="2">
         <v>1.4</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <v>2.277036324173573E-2</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="15">
         <v>0.44324983977807297</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="15">
         <v>0.48704013331596685</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="15">
         <v>4.2157077941280745</v>
       </c>
     </row>
@@ -12087,25 +12087,25 @@
       <c r="B17" s="2">
         <v>1.5</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="15">
         <v>2.0001497441423455E-3</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <v>3.8827093714842331E-2</v>
       </c>
       <c r="E17" s="2">
         <v>1.5</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <v>2.4040774420198592E-2</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="15">
         <v>0.46627001121912648</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="15">
         <v>0.46298953581092972</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="15">
         <v>4.6650644599409858</v>
       </c>
     </row>
@@ -12113,25 +12113,25 @@
       <c r="B18" s="2">
         <v>1.6</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="15">
         <v>2.002164782660628E-3</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <v>3.8850561254667196E-2</v>
       </c>
       <c r="E18" s="2">
         <v>1.6</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <v>2.657155396393919E-2</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>0.51529793420660841</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="15">
         <v>0.41919202198484223</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="15">
         <v>5.6908086475604733</v>
       </c>
     </row>
@@ -12139,25 +12139,25 @@
       <c r="B19" s="2">
         <v>1.7</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="15">
         <v>1.9990427848997098E-3</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="15">
         <v>3.8787978714324121E-2</v>
       </c>
       <c r="E19" s="2">
         <v>1.7</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <v>2.8488315935566378E-2</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="15">
         <v>0.55338152887157577</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="15">
         <v>0.38971628883619852</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="15">
         <v>6.584198015781344</v>
       </c>
     </row>
@@ -12165,25 +12165,25 @@
       <c r="B20" s="2">
         <v>1.8</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="15">
         <v>1.9997615223873032E-3</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="15">
         <v>3.8842840615393587E-2</v>
       </c>
       <c r="E20" s="2">
         <v>1.8</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="15">
         <v>3.0464742137018216E-2</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="15">
         <v>0.5916906653156353</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="15">
         <v>0.36499840157095825</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="15">
         <v>7.5061644479101624</v>
       </c>
     </row>
@@ -12191,25 +12191,25 @@
       <c r="B21" s="2">
         <v>1.9</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="15">
         <v>2.0018306474084823E-3</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="15">
         <v>3.8866304476748124E-2</v>
       </c>
       <c r="E21" s="2">
         <v>1.9</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <v>3.346457642201045E-2</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="15">
         <v>0.64929930567132155</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="15">
         <v>0.3328145798186215</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="15">
         <v>9.0280782183151818</v>
       </c>
     </row>
@@ -12217,25 +12217,25 @@
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="15">
         <v>2.0039273095510558E-3</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="15">
         <v>3.887401214283933E-2</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="15">
         <v>3.5997298812620461E-2</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="15">
         <v>0.69758671492301783</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="15">
         <v>0.3098380596931346</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="15">
         <v>10.416707548510441</v>
       </c>
     </row>
@@ -12243,25 +12243,25 @@
       <c r="B23" s="2">
         <v>2.1</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="15">
         <v>2.0025643657962692E-3</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="15">
         <v>3.8866235448411182E-2</v>
       </c>
       <c r="E23" s="2">
         <v>2.1</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="15">
         <v>3.7335836483330484E-2</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="15">
         <v>0.72462205517209544</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="15">
         <v>0.29821928150684945</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="15">
         <v>11.244199977944616</v>
       </c>
     </row>
@@ -12372,8 +12372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351BDA27-9B22-455F-BD65-EF0CD4C88C6A}">
   <dimension ref="B3:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12391,16 +12391,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="16" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
@@ -12438,25 +12438,25 @@
       <c r="B5" s="2">
         <v>0.2</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="15">
         <v>1.9997463329354884E-3</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="15">
         <v>3.8811468124265475E-2</v>
       </c>
       <c r="E5" s="2">
         <v>0.2</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="15">
         <v>1.6014301688162244E-2</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="15">
         <v>0.31163187541127996</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="15">
         <v>0.69246211664840274</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="15">
         <v>2.0854892817690454</v>
       </c>
     </row>
@@ -12464,25 +12464,25 @@
       <c r="B6" s="2">
         <v>0.3</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="15">
         <v>1.999303942313548E-3</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <v>3.8842882845335991E-2</v>
       </c>
       <c r="E6" s="2">
         <v>0.3</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <v>2.2682000745026659E-2</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <v>0.43970132865781197</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="15">
         <v>0.49116332828285109</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="15">
         <v>4.1452252292302463</v>
       </c>
     </row>
@@ -12490,25 +12490,25 @@
       <c r="B7" s="2">
         <v>0.4</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="15">
         <v>1.989384123494667E-3</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="15">
         <v>3.8600184904564599E-2</v>
       </c>
       <c r="E7" s="2">
         <v>0.4</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <v>2.8762014454542888E-2</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="15">
         <v>0.55930130029601266</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="15">
         <v>0.3837256861592131</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="15">
         <v>6.7913835334365205</v>
       </c>
     </row>
@@ -12516,25 +12516,25 @@
       <c r="B8" s="2">
         <v>0.5</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="15">
         <v>1.9837997933919941E-3</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="15">
         <v>3.8474951502813749E-2</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <v>3.513721283474782E-2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="15">
         <v>0.68157483321594259</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="15">
         <v>0.31386255199627072</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="15">
         <v>10.151284435035896</v>
       </c>
     </row>
@@ -12542,25 +12542,25 @@
       <c r="B9" s="2">
         <v>0.6</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="15">
         <v>2.0023850545011061E-3</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <v>3.8881937244317225E-2</v>
       </c>
       <c r="E9" s="2">
         <v>0.6</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <v>4.0887789149161094E-2</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="15">
         <v>0.79497649468774068</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="15">
         <v>0.27193798675577296</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="15">
         <v>13.522601315453619</v>
       </c>
     </row>
@@ -12568,25 +12568,25 @@
       <c r="B10" s="2">
         <v>0.7</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="15">
         <v>1.996412815259121E-3</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="15">
         <v>3.8725354693569906E-2</v>
       </c>
       <c r="E10" s="2">
         <v>0.7</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <v>4.5946208451044288E-2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="15">
         <v>0.89257337073647758</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="15">
         <v>0.24122815040589429</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="15">
         <v>17.184781957395909</v>
       </c>
     </row>
@@ -12594,25 +12594,25 @@
       <c r="B11" s="2">
         <v>0.8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="15">
         <v>1.9988664639107815E-3</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="15">
         <v>3.8803647087173383E-2</v>
       </c>
       <c r="E11" s="2">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <v>5.1472953933887955E-2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="15">
         <v>0.99882007765154535</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="15">
         <v>0.21600290688419166</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="15">
         <v>21.432893624591905</v>
       </c>
     </row>
@@ -12620,25 +12620,25 @@
       <c r="B12" s="2">
         <v>0.9</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="15">
         <v>2.0009446226472989E-3</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="15">
         <v>3.8834949954710769E-2</v>
       </c>
       <c r="E12" s="2">
         <v>0.9</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <v>5.6783462567340237E-2</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="15">
         <v>1.1011197726084174</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="15">
         <v>0.19609295268851726</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="15">
         <v>26.006147893759312</v>
       </c>
     </row>
@@ -12646,25 +12646,25 @@
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="15">
         <v>1.999501369459129E-3</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="15">
         <v>3.8827166987648452E-2</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>6.2276071472625143E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>1.2077878570528455</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="15">
         <v>0.17873861696526328</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="15">
         <v>31.301360451257651</v>
       </c>
     </row>
@@ -12672,25 +12672,25 @@
       <c r="B14" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="15">
         <v>2.0023371201207908E-3</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="15">
         <v>3.8874078560465812E-2</v>
       </c>
       <c r="E14" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="15">
         <v>6.7499077516462058E-2</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="15">
         <v>1.3092095058306539</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="15">
         <v>0.16509147927164389</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="15">
         <v>36.69025093871614</v>
       </c>
     </row>
@@ -12698,25 +12698,25 @@
       <c r="B15" s="2">
         <v>1.2</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="15">
         <v>1.991147076137228E-3</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="15">
         <v>3.8592252849558195E-2</v>
       </c>
       <c r="E15" s="2">
         <v>1.2</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="15">
         <v>7.2533000488097812E-2</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="15">
         <v>1.4076301290278703</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="15">
         <v>0.15243610483961614</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="15">
         <v>43.035248428070012</v>
       </c>
     </row>
@@ -12724,25 +12724,25 @@
       <c r="B16" s="2">
         <v>1.3</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="15">
         <v>2.0037806376779791E-3</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="15">
         <v>3.8874032126811328E-2</v>
       </c>
       <c r="E16" s="2">
         <v>1.3</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <v>7.7400503445711616E-2</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="15">
         <v>1.5025995258538845</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="15">
         <v>0.14384404962221839</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="15">
         <v>48.32993350456551</v>
       </c>
     </row>
@@ -12750,25 +12750,25 @@
       <c r="B17" s="2">
         <v>1.4</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="15">
         <v>2.0003921959662932E-3</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <v>3.8827124468188076E-2</v>
       </c>
       <c r="E17" s="2">
         <v>1.4</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <v>8.2221452330162398E-2</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="15">
         <v>1.5957439983140767</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="15">
         <v>0.13528407877043197</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="15">
         <v>54.639488204301351</v>
       </c>
     </row>
@@ -12776,25 +12776,25 @@
       <c r="B18" s="2">
         <v>1.5</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="15">
         <v>2.0001497441423455E-3</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <v>3.8827093714842331E-2</v>
       </c>
       <c r="E18" s="2">
         <v>1.5</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <v>8.6438548314723959E-2</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>1.6776782651247606</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="15">
         <v>0.12867696500615655</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="15">
         <v>60.394637927236445</v>
       </c>
     </row>
@@ -12802,25 +12802,25 @@
       <c r="B19" s="2">
         <v>1.6</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="15">
         <v>2.002164782660628E-3</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="15">
         <v>3.8850561254667196E-2</v>
       </c>
       <c r="E19" s="2">
         <v>1.6</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <v>9.1438471925468487E-2</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="15">
         <v>1.7753053617895729</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="15">
         <v>0.1216745298424461</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="15">
         <v>67.546157204802611</v>
       </c>
     </row>
@@ -12828,25 +12828,25 @@
       <c r="B20" s="2">
         <v>1.7</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="15">
         <v>1.9990427848997098E-3</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="15">
         <v>3.8787978714324121E-2</v>
       </c>
       <c r="E20" s="2">
         <v>1.7</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="15">
         <v>9.5982566890012236E-2</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="15">
         <v>1.8630959996070546</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="15">
         <v>0.11575430483774737</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="15">
         <v>74.632106135011924</v>
       </c>
     </row>
@@ -12854,25 +12854,25 @@
       <c r="B21" s="2">
         <v>1.8</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="15">
         <v>1.9997615223873032E-3</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="15">
         <v>3.8842840615393587E-2</v>
       </c>
       <c r="E21" s="2">
         <v>1.8</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <v>9.8898728272981157E-2</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="15">
         <v>1.9193505071523866</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="15">
         <v>0.11252020257392069</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="15">
         <v>78.983975494509224</v>
       </c>
     </row>
@@ -12880,25 +12880,25 @@
       <c r="B22" s="2">
         <v>1.9</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="15">
         <v>2.0018306474084823E-3</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="15">
         <v>3.8866304476748124E-2</v>
       </c>
       <c r="E22" s="2">
         <v>1.9</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="15">
         <v>0.10331041985020441</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="15">
         <v>2.0053936424207572</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="15">
         <v>0.10775766376287121</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="15">
         <v>86.119929531479897</v>
       </c>
     </row>
@@ -12906,25 +12906,25 @@
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="15">
         <v>2.0039273095510558E-3</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="15">
         <v>3.887401214283933E-2</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="15">
         <v>0.10708530471962889</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="15">
         <v>2.0795936685412357</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="15">
         <v>0.10393382673560407</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="15">
         <v>92.573389272382116</v>
       </c>
     </row>
@@ -12932,25 +12932,25 @@
       <c r="B24" s="2">
         <v>2.1</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="15">
         <v>2.0025643657962692E-3</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="15">
         <v>3.8866235448411182E-2</v>
       </c>
       <c r="E24" s="2">
         <v>2.1</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="15">
         <v>0.11213853597859509</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="15">
         <v>2.1779306323139536</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="15">
         <v>9.9221097717306278E-2</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="15">
         <v>101.57619610658838</v>
       </c>
     </row>
@@ -13063,16 +13063,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
@@ -13775,7 +13775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E5D255-E5BF-4A77-BC16-4DDCB08C9EC4}">
   <dimension ref="D4:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>